<commit_message>
Added pin macros and terminal control
</commit_message>
<xml_diff>
--- a/hdw/QI_Charger/QI_Charger_bom_A.xlsx
+++ b/hdw/QI_Charger/QI_Charger_bom_A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drew Maatman\Documents\KiCad Projects\Projects\QI_Charger\hdw\QI_Charger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B43D236-4FAF-4FE3-9CEB-3EC8428AA5B0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024F59BB-42DD-4CF2-9AA1-2141C407C8CC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -307,9 +307,6 @@
     <t>IPC100N04S51R7ATMA1CT-ND</t>
   </si>
   <si>
-    <t>R405 R501 R502 R701 R702 R803 R804 R1201 R1202 R1203 R1204 R1205 R1206</t>
-  </si>
-  <si>
     <t>R209 R1303</t>
   </si>
   <si>
@@ -385,9 +382,6 @@
     <t>311-1.00MHRCT-ND</t>
   </si>
   <si>
-    <t>R406 R1006 R1009 R1104 R1105 R1106 R1109 R1110 R1112 R1113 R1115 R1116 R1403</t>
-  </si>
-  <si>
     <t>1k</t>
   </si>
   <si>
@@ -701,28 +695,6 @@
   </si>
   <si>
     <t>311-0.0GRCT-ND</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>R207 R301 R308</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> R402 R404 R503 R504 R505 R506 R601 R602 R606 R703 R704 R901 R902 R903 R904 R1001 R1005 R1101 R1102 R1103 R1107 R1108 R1111 R1114 R1207 R1208 R1209 R1210 R1211 R1212 R1213 R1214 R1306 R1401 R1402 R1405 R1406 R1407</t>
-    </r>
   </si>
   <si>
     <r>
@@ -744,72 +716,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> C401 C402 C501 C502 C503 C506 C601 C602 C609 C613 C701 C807 C808 C901 C902 C1001 C1002 C1003 C1004 C1005 C1007 C1008 C1011 C1101 C1102 C1103 C1104 C1105 C1106 C1107 C1108 C1109 C1201 C1202 C1203 C1301 C1309 C1311 C1314 C1316 C1401 C1403 C1404</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>C202 C206 C302 C305</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> C504 C507 C603 C604 C607 C608 C610 C612 C614 C616 C702 C801 C802 C805 C806 C1302 C1310 C1312 C1319 C1402</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>C203 C207 C208 C306</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> C505 C508 C605 C606 C611 C615 C703 C803 C804 C1303 C1304 C1306 C1317 C1405</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>R304</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> R1304</t>
     </r>
   </si>
   <si>
@@ -874,6 +780,75 @@
   </si>
   <si>
     <t>C209 C1323</t>
+  </si>
+  <si>
+    <t>C203 C207 C208 C306 C505 C508 C605 C606 C611 C615 C703 C803 C804 C1303 C1304 C1306 C1317 C1405</t>
+  </si>
+  <si>
+    <t>C202 C206 C302 C305 C504 C507 C603 C604 C607 C608 C610 C612 C614 C616 C702 C801 C802 C805 C806 C1302 C1310 C1312 C1319 C1402</t>
+  </si>
+  <si>
+    <t>R304 R1304</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R406 R1006 R1009 R1104 R1105 R1106 R1109 R1110 R1112 R1113 R1115 R1116</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> R1403</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">R405 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R501 R502 R701 R702</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> R803 R804 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R1201 R1202 R1203 R1204 R1205 R1206</t>
+    </r>
+  </si>
+  <si>
+    <t>R207 R301 R308 R402 R404 R503 R504 R505 R506 R601 R602 R606 R703 R704 R901 R902 R903 R904 R1001 R1005 R1101 R1102 R1103 R1107 R1108 R1111 R1114 R1207 R1208 R1209 R1210 R1211 R1212 R1213 R1214 R1306 R1401 R1402 R1405 R1406 R1407</t>
   </si>
 </sst>
 </file>
@@ -1729,8 +1704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1756,7 +1731,7 @@
     </row>
     <row r="2" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -1765,12 +1740,12 @@
         <v>48</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
@@ -1783,8 +1758,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>229</v>
+      <c r="A4" s="2" t="s">
+        <v>235</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
@@ -1811,8 +1786,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>230</v>
+      <c r="A6" s="2" t="s">
+        <v>234</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>12</v>
@@ -1826,7 +1801,7 @@
     </row>
     <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>14</v>
@@ -1868,7 +1843,7 @@
     </row>
     <row r="10" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>22</v>
@@ -2232,7 +2207,7 @@
     </row>
     <row r="37" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>95</v>
+        <v>238</v>
       </c>
       <c r="B37" s="1">
         <v>0</v>
@@ -2241,12 +2216,12 @@
         <v>13</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B38" s="1">
         <v>0.02</v>
@@ -2255,12 +2230,12 @@
         <v>2</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B39" s="1">
         <v>1</v>
@@ -2269,26 +2244,26 @@
         <v>2</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="C40" s="1">
+        <v>1</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="C40" s="1">
-        <v>1</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B41" s="1">
         <v>10</v>
@@ -2297,26 +2272,26 @@
         <v>3</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="C42" s="1">
         <v>2</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B43" s="1">
         <v>100</v>
@@ -2325,124 +2300,124 @@
         <v>1</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C44" s="1">
         <v>5</v>
       </c>
       <c r="D44" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="116" x14ac:dyDescent="0.35">
+      <c r="A45" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="116" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="C45" s="1">
         <v>41</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="C46" s="1">
+        <v>1</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C46" s="1">
-        <v>1</v>
-      </c>
-      <c r="D46" s="1" t="s">
+    </row>
+    <row r="47" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A47" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="C47" s="1">
         <v>3</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="C48" s="1">
+        <v>1</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="C48" s="1">
-        <v>1</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>121</v>
+        <v>237</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C49" s="1">
         <v>13</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C50" s="1">
+        <v>1</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B50" s="1" t="s">
+    </row>
+    <row r="51" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A51" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="C50" s="1">
-        <v>1</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="C51" s="1">
         <v>2</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B52" s="1">
         <v>27</v>
@@ -2451,110 +2426,110 @@
         <v>2</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C53" s="1">
+        <v>1</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C53" s="1">
-        <v>1</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C54" s="1">
+        <v>1</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C54" s="1">
-        <v>1</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C55" s="1">
         <v>2</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C56" s="1">
+        <v>1</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C56" s="1">
-        <v>1</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C57" s="1">
+        <v>1</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C57" s="1">
-        <v>1</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C58" s="1">
+        <v>1</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C58" s="1">
-        <v>1</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C59" s="1">
+        <v>1</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B59" s="1" t="s">
+    </row>
+    <row r="60" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A60" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="C59" s="1">
-        <v>1</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A60" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="B60" s="1">
         <v>499</v>
@@ -2563,85 +2538,85 @@
         <v>6</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C61" s="1">
+        <v>1</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C61" s="1">
-        <v>1</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C62" s="1">
         <v>2</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C63" s="1">
+        <v>1</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C63" s="1">
-        <v>1</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C64" s="1">
         <v>1</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C65" s="1">
+        <v>1</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C65" s="1">
-        <v>1</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C66" s="1">
         <v>2</v>
@@ -2650,10 +2625,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C67" s="1">
         <v>1</v>
@@ -2662,220 +2637,220 @@
     </row>
     <row r="68" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C68" s="1">
         <v>1</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C69" s="1">
         <v>8</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C70" s="1">
         <v>2</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C71" s="1">
         <v>2</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C72" s="1">
         <v>4</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C73" s="1">
         <v>2</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B74" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C74" s="1">
+        <v>1</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="C74" s="1">
-        <v>1</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C75" s="1">
         <v>2</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B76" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C76" s="1">
+        <v>1</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="C76" s="1">
-        <v>1</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C77" s="1">
         <v>3</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B78" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C78" s="1">
+        <v>1</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="C78" s="1">
-        <v>1</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B79" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C79" s="1">
+        <v>1</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="C79" s="1">
-        <v>1</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B80" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C80" s="1">
+        <v>1</v>
+      </c>
+      <c r="D80" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="C80" s="1">
-        <v>1</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C81" s="1">
         <v>4</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C82" s="1">
+        <v>1</v>
+      </c>
+      <c r="D82" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C82" s="1">
-        <v>1</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C83" s="1">
         <v>1</v>
@@ -2884,47 +2859,48 @@
     </row>
     <row r="84" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A84" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B84" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C84" s="1">
+        <v>1</v>
+      </c>
+      <c r="D84" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="C84" s="1">
-        <v>1</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A85" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B85" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C85" s="1">
+        <v>1</v>
+      </c>
+      <c r="D85" s="1" t="s">
         <v>218</v>
-      </c>
-      <c r="C85" s="1">
-        <v>1</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A86" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C86" s="1">
+        <v>1</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="C86" s="1">
-        <v>1</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>223</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>